<commit_message>
initialization optimization in non-newtons
</commit_message>
<xml_diff>
--- a/pa1/results.xlsx
+++ b/pa1/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,10 +55,10 @@
     <t>Newton's opt; step=0.001</t>
   </si>
   <si>
-    <t>Newton's opt; step = 0.001</t>
+    <t>MIPS</t>
   </si>
   <si>
-    <t>MIPS</t>
+    <t>No newtons opt; step = 0.001</t>
   </si>
 </sst>
 </file>
@@ -136,6 +136,775 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No newtons opt; step = 0.001 n</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No newtons opt; step = 0.001 p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No newtons opt; step = 0.001 k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No newtons opt; step = 0.001 wtime</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>0.01692</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.011788</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.009513</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.011337</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.019098</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.066423</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.039249</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.025148</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.021169</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.032111</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.411608</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.227974</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.123033</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.079433</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.069493</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.644223</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.852103</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.466855</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.266469</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.265416</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.609898</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.485155</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.868366</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.008941</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.594752</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41.322036</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>21.235359</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11.199172</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.955222</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.185313</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>165.231836</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>84.71981</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44.498198</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>25.029599</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12.305588</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No newtons opt; step = 0.001 MIPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>5.91016548463357E7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.48320325755005E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.05119310417324E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.82067566375584E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.23615038223898E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.02201044818813E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.01913424545848E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.59058374423413E8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.88955548207284E8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.24567905079256E8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.07374006336126E7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.09661628080395E8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.03197516113563E8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.14730653506729E8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.59748463874059E8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.0819000828963E7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.17356704529851E8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.14199269580491E8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.7527817494718E8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.76767037405431E8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.05153059850545E7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.14772513704555E8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.14090815182892E8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.9645529322329E8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.7254923060368E8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.05004070951393E7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.17728172149103E8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.23230788847604E8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.19799631315172E8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.84852226453099E8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.05210245318584E7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.18036147625921E8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.24728201353232E8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.99526976041446E8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.12638940942928E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2138845640"/>
+        <c:axId val="2138482840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2138845640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2138482840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2138482840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2138845640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -463,7 +1232,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -474,7 +1243,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1"/>
       <c r="H1" s="1" t="s">
@@ -495,7 +1264,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -510,7 +1279,7 @@
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -549,143 +1318,143 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="D4">
-        <v>6.6422999999999996E-2</v>
+        <v>1.1788E-2</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E37" si="0">A4^2*C4/D4</f>
-        <v>60220104.481881283</v>
+        <f>A4^2*C4/D4</f>
+        <v>84832032.575500503</v>
       </c>
       <c r="H4">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4">
         <v>100</v>
       </c>
       <c r="K4">
-        <v>3.7595000000000003E-2</v>
+        <v>6.9849999999999999E-3</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L37" si="1">H4^2*J4/K4</f>
-        <v>106397127.2775635</v>
+        <f>H4^2*J4/K4</f>
+        <v>143163922.69148174</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
       <c r="D5">
-        <v>0.41160799999999997</v>
+        <v>9.5130000000000006E-3</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>60737400.633612566</v>
+        <f>A5^2*C5/D5</f>
+        <v>105119310.41732365</v>
       </c>
       <c r="H5">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J5">
         <v>100</v>
       </c>
       <c r="K5">
-        <v>0.23538300000000001</v>
+        <v>4.8609999999999999E-3</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
-        <v>106209879.21812534</v>
+        <f>H5^2*J5/K5</f>
+        <v>205718987.86257973</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>100</v>
       </c>
       <c r="D6">
-        <v>1.644223</v>
+        <v>1.1337E-2</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>60819000.828962982</v>
+        <f>A6^2*C6/D6</f>
+        <v>88206756.637558445</v>
       </c>
       <c r="H6">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J6">
         <v>100</v>
       </c>
       <c r="K6">
-        <v>0.94192900000000002</v>
+        <v>5.8250000000000003E-3</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
-        <v>106165114.35575293</v>
+        <f>H6^2*J6/K6</f>
+        <v>171673819.74248925</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="D7">
-        <v>6.6098980000000003</v>
+        <v>1.9098E-2</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>60515305.98505453</v>
+        <f>A7^2*C7/D7</f>
+        <v>52361503.822389781</v>
       </c>
       <c r="H7">
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J7">
         <v>100</v>
       </c>
       <c r="K7">
-        <v>4.1621920000000001</v>
+        <v>1.1709000000000001E-2</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
-        <v>96103207.156229213</v>
+        <f>H7^2*J7/K7</f>
+        <v>85404389.78563498</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -694,14 +1463,14 @@
         <v>100</v>
       </c>
       <c r="D8">
-        <v>41.322035999999997</v>
+        <v>6.6422999999999996E-2</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>60500407.095139265</v>
+        <f>A8^2*C8/D8</f>
+        <v>60220104.481881283</v>
       </c>
       <c r="H8">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -710,79 +1479,79 @@
         <v>100</v>
       </c>
       <c r="K8">
-        <v>25.995933999999998</v>
+        <v>3.7595000000000003E-2</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
-        <v>96168885.488015175</v>
+        <f>H8^2*J8/K8</f>
+        <v>106397127.2775635</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>10000</v>
+        <v>200</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>100</v>
       </c>
       <c r="D9">
-        <v>165.23183599999999</v>
+        <v>3.9248999999999999E-2</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>60521024.531858385</v>
+        <f>A9^2*C9/D9</f>
+        <v>101913424.54584831</v>
       </c>
       <c r="H9">
-        <v>10000</v>
+        <v>200</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9">
         <v>100</v>
       </c>
       <c r="K9">
-        <v>105.87946700000001</v>
+        <v>2.3434E-2</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
-        <v>94447018.702880323</v>
+        <f>H9^2*J9/K9</f>
+        <v>170692156.69539985</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>100</v>
       </c>
       <c r="D10">
-        <v>1.1788E-2</v>
+        <v>2.5148E-2</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>84832032.575500503</v>
+        <f>A10^2*C10/D10</f>
+        <v>159058374.4234134</v>
       </c>
       <c r="H10">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J10">
         <v>100</v>
       </c>
       <c r="K10">
-        <v>6.9849999999999999E-3</v>
+        <v>1.37E-2</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
-        <v>143163922.69148174</v>
+        <f>H10^2*J10/K10</f>
+        <v>291970802.91970801</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -790,106 +1559,106 @@
         <v>200</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>100</v>
       </c>
       <c r="D11">
-        <v>3.9248999999999999E-2</v>
+        <v>2.1169E-2</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>101913424.54584831</v>
+        <f>A11^2*C11/D11</f>
+        <v>188955548.20728424</v>
       </c>
       <c r="H11">
         <v>200</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J11">
         <v>100</v>
       </c>
       <c r="K11">
-        <v>2.3434E-2</v>
+        <v>1.0822999999999999E-2</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
-        <v>170692156.69539985</v>
+        <f>H11^2*J11/K11</f>
+        <v>369583294.83507347</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>100</v>
       </c>
       <c r="D12">
-        <v>0.22797400000000001</v>
+        <v>3.2111000000000001E-2</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>109661628.08039513</v>
+        <f>A12^2*C12/D12</f>
+        <v>124567905.07925633</v>
       </c>
       <c r="H12">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="J12">
         <v>100</v>
       </c>
       <c r="K12">
-        <v>0.12382899999999999</v>
+        <v>1.8884999999999999E-2</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
-        <v>201891317.8657665</v>
+        <f>H12^2*J12/K12</f>
+        <v>211808313.47630396</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>100</v>
       </c>
       <c r="D13">
-        <v>0.85210300000000005</v>
+        <v>0.41160799999999997</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>117356704.52985144</v>
+        <f>A13^2*C13/D13</f>
+        <v>60737400.633612566</v>
       </c>
       <c r="H13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <v>100</v>
       </c>
       <c r="K13">
-        <v>0.54155500000000001</v>
+        <v>0.23538300000000001</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
-        <v>184653451.63464469</v>
+        <f>H13^2*J13/K13</f>
+        <v>106209879.21812534</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -898,14 +1667,14 @@
         <v>100</v>
       </c>
       <c r="D14">
-        <v>3.4851549999999998</v>
+        <v>0.22797400000000001</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>114772513.70455547</v>
+        <f>A14^2*C14/D14</f>
+        <v>109661628.08039513</v>
       </c>
       <c r="H14">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I14">
         <v>2</v>
@@ -914,181 +1683,181 @@
         <v>100</v>
       </c>
       <c r="K14">
-        <v>2.100978</v>
+        <v>0.12382899999999999</v>
       </c>
       <c r="L14">
-        <f t="shared" si="1"/>
-        <v>190387524.28630856</v>
+        <f>H14^2*J14/K14</f>
+        <v>201891317.8657665</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>100</v>
       </c>
       <c r="D15">
-        <v>21.235358999999999</v>
+        <v>0.123033</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>117728172.14910284</v>
+        <f>A15^2*C15/D15</f>
+        <v>203197516.11356303</v>
       </c>
       <c r="H15">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J15">
         <v>100</v>
       </c>
       <c r="K15">
-        <v>13.07536</v>
+        <v>6.9862999999999995E-2</v>
       </c>
       <c r="L15">
-        <f t="shared" si="1"/>
-        <v>191199324.5310263</v>
+        <f>H15^2*J15/K15</f>
+        <v>357843207.42023677</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <v>100</v>
       </c>
       <c r="D16">
-        <v>84.719809999999995</v>
+        <v>7.9433000000000004E-2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>118036147.62592126</v>
+        <f>A16^2*C16/D16</f>
+        <v>314730653.50672895</v>
       </c>
       <c r="H16">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J16">
         <v>100</v>
       </c>
       <c r="K16">
-        <v>55.042580000000001</v>
+        <v>3.9948999999999998E-2</v>
       </c>
       <c r="L16">
-        <f t="shared" si="1"/>
-        <v>181677530.37739146</v>
+        <f>H16^2*J16/K16</f>
+        <v>625797892.31269872</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>100</v>
       </c>
       <c r="D17">
-        <v>9.5130000000000006E-3</v>
+        <v>6.9492999999999999E-2</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>105119310.41732365</v>
+        <f>A17^2*C17/D17</f>
+        <v>359748463.87405926</v>
       </c>
       <c r="H17">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="I17">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J17">
         <v>100</v>
       </c>
       <c r="K17">
-        <v>4.8609999999999999E-3</v>
+        <v>3.6790000000000003E-2</v>
       </c>
       <c r="L17">
-        <f t="shared" si="1"/>
-        <v>205718987.86257973</v>
+        <f>H17^2*J17/K17</f>
+        <v>679532481.65262294</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>100</v>
       </c>
       <c r="D18">
-        <v>2.5148E-2</v>
+        <v>1.644223</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>159058374.4234134</v>
+        <f>A18^2*C18/D18</f>
+        <v>60819000.828962982</v>
       </c>
       <c r="H18">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="I18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <v>100</v>
       </c>
       <c r="K18">
-        <v>1.37E-2</v>
+        <v>0.94192900000000002</v>
       </c>
       <c r="L18">
-        <f t="shared" si="1"/>
-        <v>291970802.91970801</v>
+        <f>H18^2*J18/K18</f>
+        <v>106165114.35575293</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>100</v>
       </c>
       <c r="D19">
-        <v>0.123033</v>
+        <v>0.85210300000000005</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>203197516.11356303</v>
+        <f>A19^2*C19/D19</f>
+        <v>117356704.52985144</v>
       </c>
       <c r="H19">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J19">
         <v>100</v>
       </c>
       <c r="K19">
-        <v>6.9862999999999995E-2</v>
+        <v>0.54155500000000001</v>
       </c>
       <c r="L19">
-        <f t="shared" si="1"/>
-        <v>357843207.42023677</v>
+        <f>H19^2*J19/K19</f>
+        <v>184653451.63464469</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1105,7 +1874,7 @@
         <v>0.46685500000000002</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f>A20^2*C20/D20</f>
         <v>214199269.58049071</v>
       </c>
       <c r="H20">
@@ -1121,183 +1890,183 @@
         <v>0.26675500000000002</v>
       </c>
       <c r="L20">
-        <f t="shared" si="1"/>
+        <f>H20^2*J20/K20</f>
         <v>374875822.38383532</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <v>100</v>
       </c>
       <c r="D21">
-        <v>1.868366</v>
+        <v>0.26646900000000001</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>214090815.18289244</v>
+        <f>A21^2*C21/D21</f>
+        <v>375278174.94717956</v>
       </c>
       <c r="H21">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J21">
         <v>100</v>
       </c>
       <c r="K21">
-        <v>1.0506009999999999</v>
+        <v>0.14386399999999999</v>
       </c>
       <c r="L21">
-        <f t="shared" si="1"/>
-        <v>380734455.80196482</v>
+        <f>H21^2*J21/K21</f>
+        <v>695100928.65484071</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>100</v>
       </c>
       <c r="D22">
-        <v>11.199172000000001</v>
+        <v>0.26541599999999999</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>223230788.84760407</v>
+        <f>A22^2*C22/D22</f>
+        <v>376767037.40543151</v>
       </c>
       <c r="H22">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="I22">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J22">
         <v>100</v>
       </c>
       <c r="K22">
-        <v>6.5876539999999997</v>
+        <v>9.0481000000000006E-2</v>
       </c>
       <c r="L22">
-        <f t="shared" si="1"/>
-        <v>379497769.61570841</v>
+        <f>H22^2*J22/K22</f>
+        <v>1105204407.5551772</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>100</v>
       </c>
       <c r="D23">
-        <v>44.498198000000002</v>
+        <v>6.6098980000000003</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>224728201.35323232</v>
+        <f>A23^2*C23/D23</f>
+        <v>60515305.98505453</v>
       </c>
       <c r="H23">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="I23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J23">
         <v>100</v>
       </c>
       <c r="K23">
-        <v>26.462826</v>
+        <v>4.1621920000000001</v>
       </c>
       <c r="L23">
-        <f t="shared" si="1"/>
-        <v>377888589.82785892</v>
+        <f>H23^2*J23/K23</f>
+        <v>96103207.156229213</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C24">
         <v>100</v>
       </c>
       <c r="D24">
-        <v>1.1337E-2</v>
+        <v>3.4851549999999998</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>88206756.637558445</v>
+        <f>A24^2*C24/D24</f>
+        <v>114772513.70455547</v>
       </c>
       <c r="H24">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="I24">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J24">
         <v>100</v>
       </c>
       <c r="K24">
-        <v>5.8250000000000003E-3</v>
+        <v>2.100978</v>
       </c>
       <c r="L24">
-        <f t="shared" si="1"/>
-        <v>171673819.74248925</v>
+        <f>H24^2*J24/K24</f>
+        <v>190387524.28630856</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="B25">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C25">
         <v>100</v>
       </c>
       <c r="D25">
-        <v>2.1169E-2</v>
+        <v>1.868366</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>188955548.20728424</v>
+        <f>A25^2*C25/D25</f>
+        <v>214090815.18289244</v>
       </c>
       <c r="H25">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="I25">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J25">
         <v>100</v>
       </c>
       <c r="K25">
-        <v>1.0822999999999999E-2</v>
+        <v>1.0506009999999999</v>
       </c>
       <c r="L25">
-        <f t="shared" si="1"/>
-        <v>369583294.83507347</v>
+        <f>H25^2*J25/K25</f>
+        <v>380734455.80196482</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="B26">
         <v>8</v>
@@ -1306,14 +2075,14 @@
         <v>100</v>
       </c>
       <c r="D26">
-        <v>7.9433000000000004E-2</v>
+        <v>1.0089410000000001</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
-        <v>314730653.50672895</v>
+        <f>A26^2*C26/D26</f>
+        <v>396455293.2232905</v>
       </c>
       <c r="H26">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="I26">
         <v>8</v>
@@ -1322,79 +2091,79 @@
         <v>100</v>
       </c>
       <c r="K26">
-        <v>3.9948999999999998E-2</v>
+        <v>0.54250299999999996</v>
       </c>
       <c r="L26">
-        <f t="shared" si="1"/>
-        <v>625797892.31269872</v>
+        <f>H26^2*J26/K26</f>
+        <v>737323111.57726324</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="B27">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C27">
         <v>100</v>
       </c>
       <c r="D27">
-        <v>0.26646900000000001</v>
+        <v>0.59475199999999995</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
-        <v>375278174.94717956</v>
+        <f>A27^2*C27/D27</f>
+        <v>672549230.60368025</v>
       </c>
       <c r="H27">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I27">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J27">
         <v>100</v>
       </c>
       <c r="K27">
-        <v>0.14386399999999999</v>
+        <v>0.29531400000000002</v>
       </c>
       <c r="L27">
-        <f t="shared" si="1"/>
-        <v>695100928.65484071</v>
+        <f>H27^2*J27/K27</f>
+        <v>1354490474.5457377</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="B28">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>100</v>
       </c>
       <c r="D28">
-        <v>1.0089410000000001</v>
+        <v>41.322035999999997</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
-        <v>396455293.2232905</v>
+        <f>A28^2*C28/D28</f>
+        <v>60500407.095139265</v>
       </c>
       <c r="H28">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="I28">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J28">
         <v>100</v>
       </c>
       <c r="K28">
-        <v>0.54250299999999996</v>
+        <v>25.995933999999998</v>
       </c>
       <c r="L28">
-        <f t="shared" si="1"/>
-        <v>737323111.57726324</v>
+        <f>H28^2*J28/K28</f>
+        <v>96168885.488015175</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1402,106 +2171,106 @@
         <v>5000</v>
       </c>
       <c r="B29">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>100</v>
       </c>
       <c r="D29">
-        <v>5.955222</v>
+        <v>21.235358999999999</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
-        <v>419799631.31517178</v>
+        <f>A29^2*C29/D29</f>
+        <v>117728172.14910284</v>
       </c>
       <c r="H29">
         <v>5000</v>
       </c>
       <c r="I29">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J29">
         <v>100</v>
       </c>
       <c r="K29">
-        <v>3.3223090000000002</v>
+        <v>13.07536</v>
       </c>
       <c r="L29">
-        <f t="shared" si="1"/>
-        <v>752488705.89701319</v>
+        <f>H29^2*J29/K29</f>
+        <v>191199324.5310263</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C30">
         <v>100</v>
       </c>
       <c r="D30">
-        <v>25.029599000000001</v>
+        <v>11.199172000000001</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
-        <v>399526976.04144597</v>
+        <f>A30^2*C30/D30</f>
+        <v>223230788.84760407</v>
       </c>
       <c r="H30">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="I30">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J30">
         <v>100</v>
       </c>
       <c r="K30">
-        <v>13.370817000000001</v>
+        <v>6.5876539999999997</v>
       </c>
       <c r="L30">
-        <f t="shared" si="1"/>
-        <v>747897454.58336616</v>
+        <f>H30^2*J30/K30</f>
+        <v>379497769.61570841</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="B31">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C31">
         <v>100</v>
       </c>
       <c r="D31">
-        <v>1.9098E-2</v>
+        <v>5.955222</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
-        <v>52361503.822389781</v>
+        <f>A31^2*C31/D31</f>
+        <v>419799631.31517178</v>
       </c>
       <c r="H31">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="I31">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J31">
         <v>100</v>
       </c>
       <c r="K31">
-        <v>1.1709000000000001E-2</v>
+        <v>3.3223090000000002</v>
       </c>
       <c r="L31">
-        <f t="shared" si="1"/>
-        <v>85404389.78563498</v>
+        <f>H31^2*J31/K31</f>
+        <v>752488705.89701319</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="B32">
         <v>16</v>
@@ -1510,14 +2279,14 @@
         <v>100</v>
       </c>
       <c r="D32">
-        <v>3.2111000000000001E-2</v>
+        <v>3.1853129999999998</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
-        <v>124567905.07925633</v>
+        <f>A32^2*C32/D32</f>
+        <v>784852226.45309901</v>
       </c>
       <c r="H32">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="I32">
         <v>16</v>
@@ -1526,147 +2295,147 @@
         <v>100</v>
       </c>
       <c r="K32">
-        <v>1.8884999999999999E-2</v>
+        <v>1.707757</v>
       </c>
       <c r="L32">
-        <f t="shared" si="1"/>
-        <v>211808313.47630396</v>
+        <f>H32^2*J32/K32</f>
+        <v>1463908506.8894463</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="B33">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>100</v>
       </c>
       <c r="D33">
-        <v>6.9492999999999999E-2</v>
+        <v>165.23183599999999</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
-        <v>359748463.87405926</v>
+        <f>A33^2*C33/D33</f>
+        <v>60521024.531858385</v>
       </c>
       <c r="H33">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="I33">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="J33">
         <v>100</v>
       </c>
       <c r="K33">
-        <v>3.6790000000000003E-2</v>
+        <v>105.87946700000001</v>
       </c>
       <c r="L33">
-        <f t="shared" si="1"/>
-        <v>679532481.65262294</v>
+        <f>H33^2*J33/K33</f>
+        <v>94447018.702880323</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="B34">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C34">
         <v>100</v>
       </c>
       <c r="D34">
-        <v>0.26541599999999999</v>
+        <v>84.719809999999995</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
-        <v>376767037.40543151</v>
+        <f>A34^2*C34/D34</f>
+        <v>118036147.62592126</v>
       </c>
       <c r="H34">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="I34">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J34">
         <v>100</v>
       </c>
       <c r="K34">
-        <v>9.0481000000000006E-2</v>
+        <v>55.042580000000001</v>
       </c>
       <c r="L34">
-        <f t="shared" si="1"/>
-        <v>1105204407.5551772</v>
+        <f>H34^2*J34/K34</f>
+        <v>181677530.37739146</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="B35">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C35">
         <v>100</v>
       </c>
       <c r="D35">
-        <v>0.59475199999999995</v>
+        <v>44.498198000000002</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
-        <v>672549230.60368025</v>
+        <f>A35^2*C35/D35</f>
+        <v>224728201.35323232</v>
       </c>
       <c r="H35">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="I35">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J35">
         <v>100</v>
       </c>
       <c r="K35">
-        <v>0.29531400000000002</v>
+        <v>26.462826</v>
       </c>
       <c r="L35">
-        <f t="shared" si="1"/>
-        <v>1354490474.5457377</v>
+        <f>H35^2*J35/K35</f>
+        <v>377888589.82785892</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="B36">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C36">
         <v>100</v>
       </c>
       <c r="D36">
-        <v>3.1853129999999998</v>
+        <v>25.029599000000001</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
-        <v>784852226.45309901</v>
+        <f>A36^2*C36/D36</f>
+        <v>399526976.04144597</v>
       </c>
       <c r="H36">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="I36">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J36">
         <v>100</v>
       </c>
       <c r="K36">
-        <v>1.707757</v>
+        <v>13.370817000000001</v>
       </c>
       <c r="L36">
-        <f t="shared" si="1"/>
-        <v>1463908506.8894463</v>
+        <f>H36^2*J36/K36</f>
+        <v>747897454.58336616</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1683,7 +2452,7 @@
         <v>12.305588</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f>A37^2*C37/D37</f>
         <v>812638940.94292772</v>
       </c>
       <c r="H37">
@@ -1699,13 +2468,17 @@
         <v>6.7276910000000001</v>
       </c>
       <c r="L37">
-        <f t="shared" si="1"/>
+        <f>H37^2*J37/K37</f>
         <v>1486394068.9309304</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="H3:L37">
+    <sortCondition ref="H3:H37"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
correct values of p for submission graph
</commit_message>
<xml_diff>
--- a/pa1/results.xlsx
+++ b/pa1/results.xlsx
@@ -136,775 +136,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$1:$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>No newtons opt; step = 0.001 n</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
-                <c:pt idx="0">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>200.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>200.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>200.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>200.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>200.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2000.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2000.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2000.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2000.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2000.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5000.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5000.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>5000.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5000.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>5000.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1:$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>No newtons opt; step = 0.001 p</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>16.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$1:$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>No newtons opt; step = 0.001 k</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
-                <c:pt idx="0">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>100.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1:$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>No newtons opt; step = 0.001 wtime</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$3:$D$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
-                <c:pt idx="0">
-                  <c:v>0.01692</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.011788</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.009513</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.011337</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.019098</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.066423</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.039249</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.025148</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.021169</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.032111</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.411608</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.227974</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.123033</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.079433</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.069493</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.644223</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.852103</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.466855</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.266469</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.265416</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6.609898</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.485155</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.868366</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.008941</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.594752</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>41.322036</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>21.235359</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>11.199172</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5.955222</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.185313</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>165.231836</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>84.71981</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44.498198</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>25.029599</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>12.305588</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$1:$E$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>No newtons opt; step = 0.001 MIPS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$3:$E$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
-                <c:pt idx="0">
-                  <c:v>5.91016548463357E7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.48320325755005E7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.05119310417324E8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.82067566375584E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.23615038223898E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.02201044818813E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.01913424545848E8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.59058374423413E8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.88955548207284E8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.24567905079256E8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.07374006336126E7</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.09661628080395E8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.03197516113563E8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.14730653506729E8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.59748463874059E8</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6.0819000828963E7</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.17356704529851E8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.14199269580491E8</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.7527817494718E8</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.76767037405431E8</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6.05153059850545E7</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.14772513704555E8</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.14090815182892E8</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.9645529322329E8</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>6.7254923060368E8</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6.05004070951393E7</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.17728172149103E8</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.23230788847604E8</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4.19799631315172E8</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7.84852226453099E8</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>6.05210245318584E7</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.18036147625921E8</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2.24728201353232E8</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.99526976041446E8</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>8.12638940942928E8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2138845640"/>
-        <c:axId val="2138482840"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="2138845640"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138482840"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2138482840"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138845640"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1232,7 +463,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2478,7 +1709,6 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>